<commit_message>
Forgot condition [ID: 11, object_selected]
</commit_message>
<xml_diff>
--- a/docs/dataset.xlsx
+++ b/docs/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kerwin Sneijders\Documents\Python\AoE2ScenarioParser\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4ADBA8-4239-4670-8775-68D827FD0D6B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7786F382-B96A-4989-8A8C-0B6E859383D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1785" windowWidth="29040" windowHeight="15840" xr2:uid="{90371F8B-6720-4A08-B900-3F8240B127A6}"/>
+    <workbookView xWindow="32175" yWindow="3510" windowWidth="25425" windowHeight="11565" activeTab="1" xr2:uid="{90371F8B-6720-4A08-B900-3F8240B127A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Effects" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="155">
   <si>
     <t>&lt;None&gt;</t>
   </si>
@@ -491,6 +491,12 @@
   </si>
   <si>
     <t>diplomacy_state</t>
+  </si>
+  <si>
+    <t>Object Selected</t>
+  </si>
+  <si>
+    <t>object_selected</t>
   </si>
 </sst>
 </file>
@@ -859,7 +865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{364BA0EA-EB89-4D86-B144-4527D89AE4FA}">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -1503,8 +1509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F646DB0-3912-400B-A816-F6F5B43556E2}">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1639,6 +1645,12 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">

</xml_diff>